<commit_message>
+ Create Interaction System and add interaction UI.
</commit_message>
<xml_diff>
--- a/Assets/Data/GameNarrative.xlsx
+++ b/Assets/Data/GameNarrative.xlsx
@@ -8,6 +8,11 @@
   </bookViews>
   <sheets>
     <sheet name="Actor" sheetId="1" r:id="rId1"/>
+    <sheet name="Dialogues" sheetId="2" r:id="rId2"/>
+    <sheet name="Lines" sheetId="3" r:id="rId3"/>
+    <sheet name="Choice" sheetId="4" r:id="rId4"/>
+    <sheet name="Quest" sheetId="5" r:id="rId5"/>
+    <sheet name="Step" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
   <si>
     <t>ID</t>
   </si>
@@ -172,6 +177,102 @@
   </si>
   <si>
     <t>STR_YANLUA_WANG</t>
+  </si>
+  <si>
+    <t>ActorID</t>
+  </si>
+  <si>
+    <t>DialogueType</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>DialogueID</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Texts</t>
+  </si>
+  <si>
+    <t>Choices</t>
+  </si>
+  <si>
+    <t>LineID</t>
+  </si>
+  <si>
+    <t>ActionChoiceType</t>
+  </si>
+  <si>
+    <t>NextDialogue</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>QusetLearm72Skill</t>
+  </si>
+  <si>
+    <t>Step01,Step02.Step03</t>
+  </si>
+  <si>
+    <t>Step01</t>
+  </si>
+  <si>
+    <t>Bồ Đề Tổ Sư</t>
+  </si>
+  <si>
+    <t>StartDialogue</t>
+  </si>
+  <si>
+    <t>Bồ Đề tổ Sư Dialogue01_ quest01_step01</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Dialogue</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>HasReward</t>
+  </si>
+  <si>
+    <t>RewardCount</t>
+  </si>
+  <si>
+    <t>Step02</t>
+  </si>
+  <si>
+    <t>Step03</t>
+  </si>
+  <si>
+    <t>Bồ Đề tổ Sư Dialogue01_ quest01_step02</t>
+  </si>
+  <si>
+    <t>Bồ Đề tổ Sư Dialogue01_ quest01_step03</t>
+  </si>
+  <si>
+    <t>GiveItem</t>
+  </si>
+  <si>
+    <t>Sư hunh đệ</t>
+  </si>
+  <si>
+    <t>CheckItem</t>
+  </si>
+  <si>
+    <t>ITEM_01</t>
+  </si>
+  <si>
+    <t>ITEM_02</t>
   </si>
 </sst>
 </file>
@@ -187,7 +288,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,6 +298,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -213,9 +320,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -501,7 +615,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,4 +815,260 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1001</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="5" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="3" width="35.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
+ Config Dialogue data.
</commit_message>
<xml_diff>
--- a/Assets/Data/GameNarrative.xlsx
+++ b/Assets/Data/GameNarrative.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Actor" sheetId="1" r:id="rId1"/>
     <sheet name="Dialogues" sheetId="2" r:id="rId2"/>
     <sheet name="Lines" sheetId="3" r:id="rId3"/>
-    <sheet name="Choice" sheetId="4" r:id="rId4"/>
-    <sheet name="Quest" sheetId="5" r:id="rId5"/>
-    <sheet name="Step" sheetId="6" r:id="rId6"/>
+    <sheet name="Choices" sheetId="4" r:id="rId4"/>
+    <sheet name="QuestLine" sheetId="7" r:id="rId5"/>
+    <sheet name="Quest" sheetId="5" r:id="rId6"/>
+    <sheet name="Step" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="85">
   <si>
     <t>ID</t>
   </si>
@@ -182,9 +183,6 @@
     <t>ActorID</t>
   </si>
   <si>
-    <t>DialogueType</t>
-  </si>
-  <si>
     <t>Default</t>
   </si>
   <si>
@@ -197,9 +195,6 @@
     <t>Texts</t>
   </si>
   <si>
-    <t>Choices</t>
-  </si>
-  <si>
     <t>LineID</t>
   </si>
   <si>
@@ -273,6 +268,18 @@
   </si>
   <si>
     <t>ITEM_02</t>
+  </si>
+  <si>
+    <t>L1_D1_Default_Dragon_king_Eatern_Sea</t>
+  </si>
+  <si>
+    <t>Default_Dragon_king</t>
+  </si>
+  <si>
+    <t>L1-D1-Default-Dragon_king</t>
+  </si>
+  <si>
+    <t>HasChoice</t>
   </si>
 </sst>
 </file>
@@ -320,12 +327,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -614,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,30 +825,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1001</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>53</v>
+      <c r="C2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -852,35 +867,53 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="5" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>57</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -893,7 +926,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,20 +939,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -929,10 +962,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,15 +993,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -962,7 +1009,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -987,36 +1034,36 @@
         <v>51</v>
       </c>
       <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>68</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>70</v>
       </c>
-      <c r="F1" t="s">
-        <v>72</v>
-      </c>
       <c r="G1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
         <v>65</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>69</v>
-      </c>
-      <c r="E2" t="s">
-        <v>71</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -1024,19 +1071,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
         <v>74</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" t="s">
         <v>79</v>
-      </c>
-      <c r="C3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" t="s">
-        <v>81</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -1047,19 +1094,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
         <v>75</v>
       </c>
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" t="s">
-        <v>77</v>
-      </c>
       <c r="D4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" t="s">
         <v>80</v>
-      </c>
-      <c r="E4" t="s">
-        <v>82</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
+ Make Dialogue of character in Game.
</commit_message>
<xml_diff>
--- a/Assets/Data/GameNarrative.xlsx
+++ b/Assets/Data/GameNarrative.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="120">
   <si>
     <t>ID</t>
   </si>
@@ -201,9 +201,6 @@
     <t>ActionChoiceType</t>
   </si>
   <si>
-    <t>NextDialogue</t>
-  </si>
-  <si>
     <t>Step</t>
   </si>
   <si>
@@ -280,6 +277,114 @@
   </si>
   <si>
     <t>HasChoice</t>
+  </si>
+  <si>
+    <t>L1_D2_Default_Dragon_king_Eatern_Sea</t>
+  </si>
+  <si>
+    <t>L1_D3_Default_Dragon_king_Eatern_Sea</t>
+  </si>
+  <si>
+    <t>DoNothing</t>
+  </si>
+  <si>
+    <t>L1-D2-Default-Dragon_king</t>
+  </si>
+  <si>
+    <t>L1-D3-Default-Dragon_king</t>
+  </si>
+  <si>
+    <t>Dia_Choice_01_Default_Wukong</t>
+  </si>
+  <si>
+    <t>Dia_Choice_03_Default_Wukong</t>
+  </si>
+  <si>
+    <t>Choice_01_Default_Wukong</t>
+  </si>
+  <si>
+    <t>Choice_03_Default_Wukong</t>
+  </si>
+  <si>
+    <t>L1_D4_Default_Dragon_king_Eatern_Sea</t>
+  </si>
+  <si>
+    <t>Dragon_king_Choice_01</t>
+  </si>
+  <si>
+    <t>Dragon_king_Choice_02</t>
+  </si>
+  <si>
+    <t>Dragon_king_Choice_03</t>
+  </si>
+  <si>
+    <t>L2-D2-Default-Dragon_king</t>
+  </si>
+  <si>
+    <t>L3-D2-Default-Dragon_king</t>
+  </si>
+  <si>
+    <t>L2_D2_Default_Dragon_king_Eatern_Sea</t>
+  </si>
+  <si>
+    <t>L3_D2_Default_Dragon_king_Eatern_Sea</t>
+  </si>
+  <si>
+    <t>L4-D2-Default-Dragon_king</t>
+  </si>
+  <si>
+    <t>L5-D2-Default-Dragon_king</t>
+  </si>
+  <si>
+    <t>L6-D2-Default-Dragon_king</t>
+  </si>
+  <si>
+    <t>L7-D2-Default-Dragon_king</t>
+  </si>
+  <si>
+    <t>L8-D2-Default-Dragon_king</t>
+  </si>
+  <si>
+    <t>L10-D2-Default-Dragon_king</t>
+  </si>
+  <si>
+    <t>L11-D2-Default-Dragon_king</t>
+  </si>
+  <si>
+    <t>L12-D2-Default-Dragon_king</t>
+  </si>
+  <si>
+    <t>L9-D2-Default-Dragon_king</t>
+  </si>
+  <si>
+    <t>L4_D2_Default_Dragon_king_Eatern_Sea</t>
+  </si>
+  <si>
+    <t>L5_D2_Default_Dragon_king_Eatern_Sea</t>
+  </si>
+  <si>
+    <t>L6_D2_Default_Dragon_king_Eatern_Sea</t>
+  </si>
+  <si>
+    <t>L7_D2_Default_Dragon_king_Eatern_Sea</t>
+  </si>
+  <si>
+    <t>L8_D2_Default_Dragon_king_Eatern_Sea</t>
+  </si>
+  <si>
+    <t>L9_D2_Default_Dragon_king_Eatern_Sea</t>
+  </si>
+  <si>
+    <t>L10_D2_Default_Dragon_king_Eatern_Sea</t>
+  </si>
+  <si>
+    <t>L11_D2_Default_Dragon_king_Eatern_Sea</t>
+  </si>
+  <si>
+    <t>L12_D2_Default_Dragon_king_Eatern_Sea</t>
+  </si>
+  <si>
+    <t>NextDialogueID</t>
   </si>
 </sst>
 </file>
@@ -621,7 +726,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,15 +930,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.140625" customWidth="1"/>
   </cols>
@@ -843,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>51</v>
@@ -851,12 +956,45 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -867,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,23 +1034,261 @@
         <v>55</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" t="b">
         <v>0</v>
       </c>
     </row>
@@ -923,19 +1299,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -952,7 +1328,41 @@
         <v>57</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>58</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -993,15 +1403,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
         <v>60</v>
-      </c>
-      <c r="B2" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1034,36 +1444,36 @@
         <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" t="s">
         <v>70</v>
-      </c>
-      <c r="G1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -1071,19 +1481,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -1094,19 +1504,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
+ Config data for the Quest Line.
</commit_message>
<xml_diff>
--- a/Assets/Data/GameNarrative.xlsx
+++ b/Assets/Data/GameNarrative.xlsx
@@ -4,16 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="Actor" sheetId="1" r:id="rId1"/>
+    <sheet name="Actors" sheetId="1" r:id="rId1"/>
     <sheet name="Dialogues" sheetId="2" r:id="rId2"/>
     <sheet name="Lines" sheetId="3" r:id="rId3"/>
     <sheet name="Choices" sheetId="4" r:id="rId4"/>
-    <sheet name="QuestLine" sheetId="7" r:id="rId5"/>
-    <sheet name="Quest" sheetId="5" r:id="rId6"/>
-    <sheet name="Step" sheetId="6" r:id="rId7"/>
+    <sheet name="QuestLines" sheetId="11" r:id="rId5"/>
+    <sheet name="Quests" sheetId="12" r:id="rId6"/>
+    <sheet name="Steps" sheetId="13" r:id="rId7"/>
+    <sheet name="Rewards" sheetId="10" r:id="rId8"/>
+    <sheet name="EventTemplate" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="161">
   <si>
     <t>ID</t>
   </si>
@@ -201,72 +203,15 @@
     <t>ActionChoiceType</t>
   </si>
   <si>
-    <t>Step</t>
-  </si>
-  <si>
-    <t>QusetLearm72Skill</t>
-  </si>
-  <si>
-    <t>Step01,Step02.Step03</t>
-  </si>
-  <si>
-    <t>Step01</t>
-  </si>
-  <si>
-    <t>Bồ Đề Tổ Sư</t>
-  </si>
-  <si>
-    <t>StartDialogue</t>
-  </si>
-  <si>
-    <t>Bồ Đề tổ Sư Dialogue01_ quest01_step01</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
     <t>Dialogue</t>
   </si>
   <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Null</t>
-  </si>
-  <si>
     <t>HasReward</t>
   </si>
   <si>
-    <t>RewardCount</t>
-  </si>
-  <si>
-    <t>Step02</t>
-  </si>
-  <si>
-    <t>Step03</t>
-  </si>
-  <si>
-    <t>Bồ Đề tổ Sư Dialogue01_ quest01_step02</t>
-  </si>
-  <si>
-    <t>Bồ Đề tổ Sư Dialogue01_ quest01_step03</t>
-  </si>
-  <si>
-    <t>GiveItem</t>
-  </si>
-  <si>
-    <t>Sư hunh đệ</t>
-  </si>
-  <si>
-    <t>CheckItem</t>
-  </si>
-  <si>
-    <t>ITEM_01</t>
-  </si>
-  <si>
-    <t>ITEM_02</t>
-  </si>
-  <si>
     <t>L1_D1_Default_Dragon_king_Eatern_Sea</t>
   </si>
   <si>
@@ -385,6 +330,186 @@
   </si>
   <si>
     <t>NextDialogueID</t>
+  </si>
+  <si>
+    <t>Payload Template (JSON)</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>{"ItemID: "Exp", "Quantity": 1}</t>
+  </si>
+  <si>
+    <t>Điền Item ID và số lượng</t>
+  </si>
+  <si>
+    <t>ITEM_PICKUP</t>
+  </si>
+  <si>
+    <t>Description Action</t>
+  </si>
+  <si>
+    <t>Nhặt item, thu thập quest item</t>
+  </si>
+  <si>
+    <t>NPC_TALK</t>
+  </si>
+  <si>
+    <t>{"ActorID:"NPC"}</t>
+  </si>
+  <si>
+    <t>Diền ID của NPC</t>
+  </si>
+  <si>
+    <t>Nói chuyện với NPC</t>
+  </si>
+  <si>
+    <t>LOCATION_ENTER</t>
+  </si>
+  <si>
+    <t>{"LcoationID":"ID"}</t>
+  </si>
+  <si>
+    <t>Điền ID của vùng or map</t>
+  </si>
+  <si>
+    <t>Vào vùng/map mới</t>
+  </si>
+  <si>
+    <t>USE_ITEM</t>
+  </si>
+  <si>
+    <t>QUEST_COMPLELET</t>
+  </si>
+  <si>
+    <t>{"Quest":"ID"}</t>
+  </si>
+  <si>
+    <t>Điền ID của quest</t>
+  </si>
+  <si>
+    <t>Hoàn tất quest</t>
+  </si>
+  <si>
+    <t>DIALOGUE_CHOICE</t>
+  </si>
+  <si>
+    <t>{"ActorID":"ID", "ChoiceID":"ID"}</t>
+  </si>
+  <si>
+    <t>Điền NPC ID</t>
+  </si>
+  <si>
+    <t>{"ItemID":"ID", "TargetID": "ID"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Điền ItemID và targetID </t>
+  </si>
+  <si>
+    <t>Sử dụng vật phẩm cho nv chính or NPC</t>
+  </si>
+  <si>
+    <t>Người chơi chọn option trong đối thoại</t>
+  </si>
+  <si>
+    <t>ENEMY_DEFEATED</t>
+  </si>
+  <si>
+    <t>Giết quái hoàn thành nhiệm vụ</t>
+  </si>
+  <si>
+    <t>TIME_EVENT</t>
+  </si>
+  <si>
+    <t>{monsterId, count}</t>
+  </si>
+  <si>
+    <t>{hour, minute}</t>
+  </si>
+  <si>
+    <t>CUTSCENE_TRIGGER</t>
+  </si>
+  <si>
+    <t>{sceneId}</t>
+  </si>
+  <si>
+    <t>Kích hoạt cinematic</t>
+  </si>
+  <si>
+    <t>Thời gian trong game thay đổi</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>QuestLineID</t>
+  </si>
+  <si>
+    <t>ItemID</t>
+  </si>
+  <si>
+    <t>RewardID</t>
+  </si>
+  <si>
+    <t>ACHIEVEMENT_UNLOCKED</t>
+  </si>
+  <si>
+    <t>{achievementId}</t>
+  </si>
+  <si>
+    <t>Mở thành tựa game</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Default_01</t>
+  </si>
+  <si>
+    <t>Tofu_Soup</t>
+  </si>
+  <si>
+    <t>Jade</t>
+  </si>
+  <si>
+    <t>Coin</t>
+  </si>
+  <si>
+    <t>QUEST_REWARD</t>
+  </si>
+  <si>
+    <t>{"rewardItems":[{"itemId":101,"count":1},{"itemId":102,"count":5}],"exp":100,"gold":50}</t>
+  </si>
+  <si>
+    <t>Nhận được reweard khi hoàn thành quest</t>
+  </si>
+  <si>
+    <t>Default_QuestLine_Name</t>
+  </si>
+  <si>
+    <t>Default_QuestLine_Description</t>
+  </si>
+  <si>
+    <t>Default_Quest_Name</t>
+  </si>
+  <si>
+    <t>Default_Quest_Description</t>
+  </si>
+  <si>
+    <t>EventID</t>
+  </si>
+  <si>
+    <t>DialogueBeforeStep</t>
+  </si>
+  <si>
+    <t>CompleteDialogue</t>
+  </si>
+  <si>
+    <t>IncompleteDialogue</t>
+  </si>
+  <si>
+    <t>QuestID</t>
   </si>
 </sst>
 </file>
@@ -432,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -442,6 +567,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -726,7 +855,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,22 +1070,26 @@
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>52</v>
@@ -965,9 +1098,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>52</v>
@@ -976,9 +1109,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>52</v>
@@ -987,9 +1120,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>52</v>
@@ -1007,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,21 +1167,21 @@
         <v>55</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -1056,16 +1189,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -1073,16 +1206,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -1090,16 +1223,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -1107,16 +1240,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -1124,16 +1257,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -1141,16 +1274,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -1158,16 +1291,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -1175,16 +1308,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -1192,16 +1325,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -1209,16 +1342,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -1226,16 +1359,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -1243,16 +1376,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
         <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -1260,16 +1393,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -1277,16 +1410,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -1302,7 +1435,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,41 +1461,41 @@
         <v>57</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1372,21 +1505,54 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1394,25 +1560,44 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
-    <col min="2" max="3" width="35.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="C2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1421,108 +1606,326 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>146</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="3">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" customWidth="1"/>
+    <col min="5" max="7" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>113</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ Add class quest manager.
</commit_message>
<xml_diff>
--- a/Assets/Data/GameNarrative.xlsx
+++ b/Assets/Data/GameNarrative.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="167">
   <si>
     <t>ID</t>
   </si>
@@ -510,6 +510,24 @@
   </si>
   <si>
     <t>QuestID</t>
+  </si>
+  <si>
+    <t>Nomarl</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Start_Quest_Dragon_king</t>
+  </si>
+  <si>
+    <t>Default-Dragon_king</t>
+  </si>
+  <si>
+    <t>L_Deafult_Dragon_king_Eatern_Sea</t>
   </si>
 </sst>
 </file>
@@ -1059,15 +1077,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.140625" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
@@ -1103,7 +1121,7 @@
         <v>75</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>52</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
@@ -1114,7 +1132,7 @@
         <v>76</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>52</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -1125,9 +1143,20 @@
         <v>77</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1138,7 +1167,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
@@ -1175,7 +1204,7 @@
         <v>63</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>164</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -1422,6 +1451,23 @@
         <v>99</v>
       </c>
       <c r="E16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E17" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1555,7 +1601,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,8 +1654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1617,7 +1663,7 @@
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -1671,7 +1717,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>62</v>
+        <v>164</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -1698,7 +1744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
+ Create Battle Scene and Create Battel State System Manager.
</commit_message>
<xml_diff>
--- a/Assets/Data/GameNarrative.xlsx
+++ b/Assets/Data/GameNarrative.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="1" r:id="rId1"/>
     <sheet name="Dialogues" sheetId="2" r:id="rId2"/>
     <sheet name="Lines" sheetId="3" r:id="rId3"/>
     <sheet name="Choices" sheetId="4" r:id="rId4"/>
-    <sheet name="QuestLines" sheetId="11" r:id="rId5"/>
-    <sheet name="Quests" sheetId="12" r:id="rId6"/>
-    <sheet name="Steps" sheetId="13" r:id="rId7"/>
-    <sheet name="Rewards" sheetId="10" r:id="rId8"/>
-    <sheet name="EventTemplate" sheetId="8" r:id="rId9"/>
+    <sheet name="DailyQuests" sheetId="14" r:id="rId5"/>
+    <sheet name="Achievements" sheetId="15" r:id="rId6"/>
+    <sheet name="QuestLines" sheetId="11" r:id="rId7"/>
+    <sheet name="Quests" sheetId="12" r:id="rId8"/>
+    <sheet name="Steps" sheetId="13" r:id="rId9"/>
+    <sheet name="Rewards" sheetId="10" r:id="rId10"/>
+    <sheet name="EventTemplate" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="171">
   <si>
     <t>ID</t>
   </si>
@@ -528,6 +530,18 @@
   </si>
   <si>
     <t>L_Deafult_Dragon_king_Eatern_Sea</t>
+  </si>
+  <si>
+    <t>Reward</t>
+  </si>
+  <si>
+    <t>Talk</t>
+  </si>
+  <si>
+    <t>Collect</t>
+  </si>
+  <si>
+    <t>Kill</t>
   </si>
 </sst>
 </file>
@@ -873,7 +887,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,6 +1082,245 @@
       </c>
       <c r="C17" t="s">
         <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="3">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" customWidth="1"/>
+    <col min="5" max="7" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1481,7 +1734,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,10 +1804,78 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,18 +1917,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
@@ -1650,12 +1971,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,243 +2059,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C4" s="3">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" customWidth="1"/>
-    <col min="5" max="7" width="27" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>121</v>
-      </c>
-      <c r="B7" t="s">
-        <v>122</v>
-      </c>
-      <c r="C7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B8" t="s">
-        <v>131</v>
-      </c>
-      <c r="D8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" t="s">
-        <v>132</v>
-      </c>
-      <c r="D9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>133</v>
-      </c>
-      <c r="B10" t="s">
-        <v>134</v>
-      </c>
-      <c r="D10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B11" t="s">
-        <v>142</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B12" t="s">
-        <v>150</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>